<commit_message>
adding WebEventListener and general enhancements
</commit_message>
<xml_diff>
--- a/Resources/TestData/ControlFile.xlsx
+++ b/Resources/TestData/ControlFile.xlsx
@@ -211,22 +211,22 @@
     <t>Jenkins</t>
   </si>
   <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>Validate Add New User</t>
+  </si>
+  <si>
+    <t>JenKin_001</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>demo1</t>
+  </si>
+  <si>
     <t>http://localhost:8080/login</t>
-  </si>
-  <si>
-    <t>Execution</t>
-  </si>
-  <si>
-    <t>Validate Add New User</t>
-  </si>
-  <si>
-    <t>JenKin_001</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>demo1</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1085,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1115,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>58</v>
@@ -1394,7 +1394,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -1497,10 +1497,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1591,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="28"/>
       <c r="H2" s="28"/>

</xml_diff>

<commit_message>
"update the example to codewars website"
</commit_message>
<xml_diff>
--- a/Resources/TestData/ControlFile.xlsx
+++ b/Resources/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="5130" tabRatio="919"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="5130" tabRatio="919" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="14" r:id="rId1"/>
@@ -226,7 +226,7 @@
     <t>demo1</t>
   </si>
   <si>
-    <t>http://localhost:8080/login</t>
+    <t>https://www.codewars.com/users/sign_in</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -540,6 +540,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1084,8 +1087,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1335,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1457,10 +1460,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,6 +1505,9 @@
       <c r="C3" s="36" t="s">
         <v>65</v>
       </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="15" t="b">
         <v>1</v>

</xml_diff>